<commit_message>
Optimized reading in tallyChars02. Reading is now done in chunks of 256 bytes. Massive improvement.
</commit_message>
<xml_diff>
--- a/3/stats.xlsx
+++ b/3/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claus\CloudStation\Bsc 2020\2 semester\UFO\assignments\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88033A75-5478-4796-A7B5-BF7EAE91ECEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036BFBCB-FB89-4FA1-A695-F79BD6A2D359}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{5E9229CC-A040-4246-8326-3BDBB72CFE23}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>n</t>
   </si>
@@ -58,6 +58,45 @@
   </si>
   <si>
     <t>MADS</t>
+  </si>
+  <si>
+    <t>doWork01</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70,2 29,348 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,8  2,386 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,3  1,941 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  40,3  1,841 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,9  1,976 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  40,1  1,612 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,5  2,444 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,3  1,635 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  40,0  2,716 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,2  1,319 </t>
   </si>
 </sst>
 </file>
@@ -110,6 +149,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>123124</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>94952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Billede 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8453F24C-ECAF-488E-8E46-49E53056765C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315200" y="1524000"/>
+          <a:ext cx="5609524" cy="2380952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5537C0-A1AC-42A2-AF01-8D3FF27D9192}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A21" sqref="A21:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,197 +521,379 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E7" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H8" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>185.2</v>
-      </c>
-      <c r="B6">
-        <v>61.216000000000001</v>
-      </c>
-      <c r="C6">
-        <v>215.3</v>
-      </c>
-      <c r="D6">
-        <v>61.594999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>150.19999999999999</v>
-      </c>
-      <c r="B7">
-        <v>12.432</v>
-      </c>
-      <c r="C7">
-        <v>155.9</v>
-      </c>
-      <c r="D7">
-        <v>7.2949999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>150.5</v>
-      </c>
-      <c r="B8">
-        <v>12.079000000000001</v>
-      </c>
-      <c r="C8">
-        <v>171.5</v>
-      </c>
-      <c r="D8">
-        <v>12.265000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>148.30000000000001</v>
+        <v>150.1</v>
       </c>
       <c r="B9">
-        <v>11.731</v>
+        <v>62.343000000000004</v>
       </c>
       <c r="C9">
-        <v>172.5</v>
+        <v>109</v>
       </c>
       <c r="D9">
-        <v>6.5919999999999996</v>
+        <v>34.887</v>
+      </c>
+      <c r="E9">
+        <v>92.6</v>
+      </c>
+      <c r="F9">
+        <v>33.999000000000002</v>
+      </c>
+      <c r="G9">
+        <v>66.2</v>
+      </c>
+      <c r="H9">
+        <v>13.76</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>201.9</v>
+        <v>106</v>
       </c>
       <c r="B10">
-        <v>6.5330000000000004</v>
+        <v>1.9239999999999999</v>
       </c>
       <c r="C10">
-        <v>190.5</v>
+        <v>75</v>
       </c>
       <c r="D10">
-        <v>26.184000000000001</v>
+        <v>3.0430000000000001</v>
+      </c>
+      <c r="E10">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="F10">
+        <v>4.3049999999999997</v>
+      </c>
+      <c r="G10">
+        <v>60</v>
+      </c>
+      <c r="H10">
+        <v>3.8889999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>186.9</v>
+        <v>108.7</v>
       </c>
       <c r="B11">
-        <v>27.027000000000001</v>
+        <v>3.4369999999999998</v>
       </c>
       <c r="C11">
-        <v>194</v>
+        <v>78.8</v>
       </c>
       <c r="D11">
-        <v>14.678000000000001</v>
+        <v>8.8620000000000001</v>
+      </c>
+      <c r="E11">
+        <v>65.5</v>
+      </c>
+      <c r="F11">
+        <v>2.391</v>
+      </c>
+      <c r="G11">
+        <v>58</v>
+      </c>
+      <c r="H11">
+        <v>1.4790000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>150.6</v>
+        <v>107.5</v>
       </c>
       <c r="B12">
-        <v>11.87</v>
+        <v>3.3319999999999999</v>
       </c>
       <c r="C12">
-        <v>170.8</v>
+        <v>100.9</v>
       </c>
       <c r="D12">
-        <v>14.843</v>
+        <v>2.6789999999999998</v>
+      </c>
+      <c r="E12">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="F12">
+        <v>7.6210000000000004</v>
+      </c>
+      <c r="G12">
+        <v>58.9</v>
+      </c>
+      <c r="H12">
+        <v>2.1120000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>147.9</v>
+        <v>107.3</v>
       </c>
       <c r="B13">
-        <v>11.462</v>
+        <v>3.4209999999999998</v>
       </c>
       <c r="C13">
-        <v>158.6</v>
+        <v>103</v>
       </c>
       <c r="D13">
-        <v>22.713000000000001</v>
+        <v>6.6909999999999998</v>
+      </c>
+      <c r="E13">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="F13">
+        <v>1.631</v>
+      </c>
+      <c r="G13">
+        <v>58</v>
+      </c>
+      <c r="H13">
+        <v>1.806</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>148.5</v>
+        <v>112.1</v>
       </c>
       <c r="B14">
-        <v>11.919</v>
+        <v>13.55</v>
       </c>
       <c r="C14">
-        <v>173.2</v>
+        <v>72.8</v>
       </c>
       <c r="D14">
-        <v>24.346</v>
+        <v>3.0779999999999998</v>
+      </c>
+      <c r="E14">
+        <v>64.2</v>
+      </c>
+      <c r="F14">
+        <v>1.6040000000000001</v>
+      </c>
+      <c r="G14">
+        <v>57.8</v>
+      </c>
+      <c r="H14">
+        <v>0.70299999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>149.19999999999999</v>
+        <v>107.9</v>
       </c>
       <c r="B15">
-        <v>11.096</v>
+        <v>2.4140000000000001</v>
       </c>
       <c r="C15">
-        <v>190.8</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="D15">
-        <v>27.721</v>
+        <v>3.98</v>
+      </c>
+      <c r="E15">
+        <v>63.9</v>
+      </c>
+      <c r="F15">
+        <v>2.4129999999999998</v>
+      </c>
+      <c r="G15">
+        <v>57.7</v>
+      </c>
+      <c r="H15">
+        <v>1.6020000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>107.3</v>
+      </c>
+      <c r="B16">
+        <v>2.794</v>
+      </c>
+      <c r="C16">
+        <v>75.2</v>
+      </c>
+      <c r="D16">
+        <v>2.6560000000000001</v>
+      </c>
+      <c r="E16">
+        <v>65</v>
+      </c>
+      <c r="F16">
+        <v>2.3959999999999999</v>
+      </c>
+      <c r="G16">
+        <v>58.1</v>
+      </c>
+      <c r="H16">
+        <v>1.4330000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>126.6</v>
+      </c>
+      <c r="B17">
+        <v>19.302</v>
+      </c>
+      <c r="C17">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D17">
+        <v>2.1720000000000002</v>
+      </c>
+      <c r="E17">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="F17">
+        <v>2.02</v>
+      </c>
+      <c r="G17">
+        <v>56.2</v>
+      </c>
+      <c r="H17">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>127.7</v>
+      </c>
+      <c r="B18">
+        <v>21.052</v>
+      </c>
+      <c r="C18">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="D18">
+        <v>3.6</v>
+      </c>
+      <c r="E18">
+        <v>67.3</v>
+      </c>
+      <c r="F18">
+        <v>3.036</v>
+      </c>
+      <c r="G18">
+        <v>56.6</v>
+      </c>
+      <c r="H18">
+        <v>1.2310000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Improvement done with BufferedInputStream.
</commit_message>
<xml_diff>
--- a/3/stats.xlsx
+++ b/3/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claus\CloudStation\Bsc 2020\2 semester\UFO\assignments\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036BFBCB-FB89-4FA1-A695-F79BD6A2D359}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC19C23-CC84-4E47-939B-38A8D4D5379E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{5E9229CC-A040-4246-8326-3BDBB72CFE23}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>n</t>
   </si>
@@ -69,34 +69,43 @@
     <t>Windows</t>
   </si>
   <si>
-    <t xml:space="preserve">70,2 29,348 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,8  2,386 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,3  1,941 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  40,3  1,841 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,9  1,976 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  40,1  1,612 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,5  2,444 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,3  1,635 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  40,0  2,716 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,2  1,319 </t>
+    <t>doWork02</t>
+  </si>
+  <si>
+    <t>doWork03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79,7 41,216 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  46,1 12,232 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  40,3  2,094 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  40,3  1,963 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,8  2,117 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,9  2,769 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,6  1,814 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,7  1,165 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  40,0  3,097 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  39,3  1,384 </t>
+  </si>
+  <si>
+    <t>(byte arrays med 128 eller 256 pladser formentlig bedst.)</t>
   </si>
 </sst>
 </file>
@@ -497,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5537C0-A1AC-42A2-AF01-8D3FF27D9192}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,54 +849,327 @@
         <v>1.2310000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>11</v>
       </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22">
+        <v>70.2</v>
+      </c>
+      <c r="B22">
+        <v>29.347999999999999</v>
+      </c>
+      <c r="C22">
+        <v>47.4</v>
+      </c>
+      <c r="D22">
+        <v>16.309000000000001</v>
+      </c>
+      <c r="E22">
+        <v>57</v>
+      </c>
+      <c r="F22">
+        <v>38.256999999999998</v>
+      </c>
+      <c r="G22">
+        <v>28.3</v>
+      </c>
+      <c r="H22">
+        <v>14.875</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="B23">
+        <v>2.3860000000000001</v>
+      </c>
+      <c r="C23">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="D23">
+        <v>1.591</v>
+      </c>
+      <c r="E23">
+        <v>24.1</v>
+      </c>
+      <c r="F23">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="G23">
+        <v>21.7</v>
+      </c>
+      <c r="H23">
+        <v>3.0089999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="B24">
+        <v>1.9410000000000001</v>
+      </c>
+      <c r="C24">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="D24">
+        <v>1.23</v>
+      </c>
+      <c r="E24">
+        <v>25.5</v>
+      </c>
+      <c r="F24">
+        <v>6.3079999999999998</v>
+      </c>
+      <c r="G24">
+        <v>21.7</v>
+      </c>
+      <c r="H24">
+        <v>2.113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="B25">
+        <v>1.841</v>
+      </c>
+      <c r="C25">
+        <v>36.4</v>
+      </c>
+      <c r="D25">
+        <v>1.7</v>
+      </c>
+      <c r="E25">
+        <v>23.3</v>
+      </c>
+      <c r="F25">
+        <v>1.6930000000000001</v>
+      </c>
+      <c r="G25">
+        <v>20.2</v>
+      </c>
+      <c r="H25">
+        <v>2.0430000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>39.9</v>
+      </c>
+      <c r="B26">
+        <v>1.976</v>
+      </c>
+      <c r="C26">
+        <v>36.1</v>
+      </c>
+      <c r="D26">
+        <v>1.337</v>
+      </c>
+      <c r="E26">
+        <v>24</v>
+      </c>
+      <c r="F26">
+        <v>2.1459999999999999</v>
+      </c>
+      <c r="G26">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="H26">
+        <v>0.80500000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>40.1</v>
+      </c>
+      <c r="B27">
+        <v>1.6120000000000001</v>
+      </c>
+      <c r="C27">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="D27">
+        <v>2.13</v>
+      </c>
+      <c r="E27">
+        <v>25.2</v>
+      </c>
+      <c r="F27">
+        <v>3.0710000000000002</v>
+      </c>
+      <c r="G27">
+        <v>21.2</v>
+      </c>
+      <c r="H27">
+        <v>2.0379999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>39.5</v>
+      </c>
+      <c r="B28">
+        <v>2.444</v>
+      </c>
+      <c r="C28">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="D28">
+        <v>1.228</v>
+      </c>
+      <c r="E28">
+        <v>22.7</v>
+      </c>
+      <c r="F28">
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="G28">
+        <v>20.2</v>
+      </c>
+      <c r="H28">
+        <v>1.4419999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="B29">
+        <v>1.635</v>
+      </c>
+      <c r="C29">
+        <v>36.6</v>
+      </c>
+      <c r="D29">
+        <v>1.319</v>
+      </c>
+      <c r="E29">
+        <v>21.8</v>
+      </c>
+      <c r="F29">
+        <v>2.286</v>
+      </c>
+      <c r="G29">
+        <v>20.3</v>
+      </c>
+      <c r="H29">
+        <v>1.278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>40</v>
+      </c>
+      <c r="B30">
+        <v>2.7160000000000002</v>
+      </c>
+      <c r="C30">
+        <v>36.4</v>
+      </c>
+      <c r="D30">
+        <v>1.339</v>
+      </c>
+      <c r="E30">
+        <v>22.3</v>
+      </c>
+      <c r="F30">
+        <v>1.8959999999999999</v>
+      </c>
+      <c r="G30">
+        <v>21.1</v>
+      </c>
+      <c r="H30">
+        <v>4.4080000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="B31">
+        <v>1.319</v>
+      </c>
+      <c r="C31">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="D31">
+        <v>2.5459999999999998</v>
+      </c>
+      <c r="E31">
+        <v>22.2</v>
+      </c>
+      <c r="F31">
+        <v>1.3080000000000001</v>
+      </c>
+      <c r="G31">
+        <v>22.3</v>
+      </c>
+      <c r="H31">
+        <v>6.4980000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimization complete, documentation pending.
</commit_message>
<xml_diff>
--- a/3/stats.xlsx
+++ b/3/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claus\CloudStation\Bsc 2020\2 semester\UFO\assignments\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC19C23-CC84-4E47-939B-38A8D4D5379E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6A8A28-26BC-4471-B3A3-D8F6F7FCF576}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{5E9229CC-A040-4246-8326-3BDBB72CFE23}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>n</t>
   </si>
@@ -75,37 +75,10 @@
     <t>doWork03</t>
   </si>
   <si>
-    <t xml:space="preserve">79,7 41,216 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  46,1 12,232 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  40,3  2,094 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  40,3  1,963 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,8  2,117 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,9  2,769 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,6  1,814 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,7  1,165 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  40,0  3,097 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  39,3  1,384 </t>
-  </si>
-  <si>
     <t>(byte arrays med 128 eller 256 pladser formentlig bedst.)</t>
+  </si>
+  <si>
+    <t>Buffered Input Stream</t>
   </si>
 </sst>
 </file>
@@ -508,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5537C0-A1AC-42A2-AF01-8D3FF27D9192}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34:G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +827,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1117,59 +1090,272 @@
         <v>6.4980000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B33" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>22</v>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>94.4</v>
+      </c>
+      <c r="B34">
+        <v>34.442</v>
+      </c>
+      <c r="C34">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="D34">
+        <v>11.295</v>
+      </c>
+      <c r="E34">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="F34">
+        <v>27.286000000000001</v>
+      </c>
+      <c r="G34">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="H34">
+        <v>10.292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>65.7</v>
+      </c>
+      <c r="B35">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C35">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="D35">
+        <v>10.275</v>
+      </c>
+      <c r="E35">
+        <v>58.7</v>
+      </c>
+      <c r="F35">
+        <v>17.66</v>
+      </c>
+      <c r="G35">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="H35">
+        <v>0.53800000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="B36">
+        <v>2.4529999999999998</v>
+      </c>
+      <c r="C36">
+        <v>36.5</v>
+      </c>
+      <c r="D36">
+        <v>0.47</v>
+      </c>
+      <c r="E36">
+        <v>42.7</v>
+      </c>
+      <c r="F36">
+        <v>2.101</v>
+      </c>
+      <c r="G36">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="H36">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="B37">
+        <v>2.1720000000000002</v>
+      </c>
+      <c r="C37">
+        <v>36.6</v>
+      </c>
+      <c r="D37">
+        <v>1.7509999999999999</v>
+      </c>
+      <c r="E37">
+        <v>47</v>
+      </c>
+      <c r="F37">
+        <v>7.7279999999999998</v>
+      </c>
+      <c r="G37">
+        <v>34.5</v>
+      </c>
+      <c r="H37">
+        <v>0.61599999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>65.3</v>
+      </c>
+      <c r="B38">
+        <v>2.375</v>
+      </c>
+      <c r="C38">
+        <v>36.6</v>
+      </c>
+      <c r="D38">
+        <v>1.53</v>
+      </c>
+      <c r="E38">
+        <v>46.7</v>
+      </c>
+      <c r="F38">
+        <v>13.627000000000001</v>
+      </c>
+      <c r="G38">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="H38">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>65.3</v>
+      </c>
+      <c r="B39">
+        <v>2.101</v>
+      </c>
+      <c r="C39">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="D39">
+        <v>1.65</v>
+      </c>
+      <c r="E39">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="F39">
+        <v>2.056</v>
+      </c>
+      <c r="G39">
+        <v>34.6</v>
+      </c>
+      <c r="H39">
+        <v>0.60699999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>67.3</v>
+      </c>
+      <c r="B40">
+        <v>3.8260000000000001</v>
+      </c>
+      <c r="C40">
+        <v>36</v>
+      </c>
+      <c r="D40">
+        <v>1.1819999999999999</v>
+      </c>
+      <c r="E40">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="F40">
+        <v>1.6120000000000001</v>
+      </c>
+      <c r="G40">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="H40">
+        <v>0.49299999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="B41">
+        <v>1.357</v>
+      </c>
+      <c r="C41">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="D41">
+        <v>1.3340000000000001</v>
+      </c>
+      <c r="E41">
+        <v>39.9</v>
+      </c>
+      <c r="F41">
+        <v>1.2</v>
+      </c>
+      <c r="G41">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="H41">
+        <v>0.59799999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>65.8</v>
+      </c>
+      <c r="B42">
+        <v>1.7150000000000001</v>
+      </c>
+      <c r="C42">
+        <v>36.1</v>
+      </c>
+      <c r="D42">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="E42">
+        <v>39.9</v>
+      </c>
+      <c r="F42">
+        <v>1.6850000000000001</v>
+      </c>
+      <c r="G42">
+        <v>34.6</v>
+      </c>
+      <c r="H42">
+        <v>0.56799999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="B43">
+        <v>2.218</v>
+      </c>
+      <c r="C43">
+        <v>36.4</v>
+      </c>
+      <c r="D43">
+        <v>1.359</v>
+      </c>
+      <c r="E43">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="F43">
+        <v>2.8029999999999999</v>
+      </c>
+      <c r="G43">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="H43">
+        <v>0.70299999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>